<commit_message>
First draft comments on mapping MedicationDispense
</commit_message>
<xml_diff>
--- a/zibs2024/mappable/nl.zorg.MedicationDispense-v3.0.1(2024EN).xlsx
+++ b/zibs2024/mappable/nl.zorg.MedicationDispense-v3.0.1(2024EN).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nictiznl.sharepoint.com/sites/ZIBcentrum2/Gedeelde  documenten/9. Overig/9.13 Xt-EHR logical models vergelijking/zibs2024/mappable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nictiznl-my.sharepoint.com/personal/wouter_zanen_nictiz_nl/Documents/Documenten/GitHub/eu-nl-compared/zibs2024/mappable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_9BE1D8B38F95E781E365EBF552BA0676B0F8E77E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04AC125A-7E77-4B8B-AD7E-277EA1464637}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_9BE1D8B38F95E781E365EBF552BA0676B0F8E77E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD2401AA-2366-4D84-8F13-976BB3A87056}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -632,18 +632,18 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.77734375" customWidth="1"/>
-    <col min="2" max="2" width="57.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" customWidth="1"/>
-    <col min="8" max="8" width="39.77734375" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -695,7 +695,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -718,7 +718,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -741,7 +741,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -764,7 +764,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -790,7 +790,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -816,7 +816,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -842,7 +842,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -868,7 +868,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -894,7 +894,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -920,7 +920,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -946,7 +946,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1235,6 +1235,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="3af30693-c405-4a5b-908a-bd1dc294f76b" xsi:nil="true"/>
@@ -1244,15 +1253,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1275,6 +1275,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AD467BC-8ECE-43DC-91C2-1F49256F0A0A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C14C2B1D-38DB-415E-8DA8-AF8D6D22C998}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1283,12 +1291,4 @@
     <ds:schemaRef ds:uri="b19602bd-a67a-4df8-b412-b401dd608f7a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AD467BC-8ECE-43DC-91C2-1F49256F0A0A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>